<commit_message>
Changed template for client name input
</commit_message>
<xml_diff>
--- a/assets/frequency_report_template.xlsx
+++ b/assets/frequency_report_template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natashasoldin/Documents/Work/Sunrise Frequency Reporting/Sunrise-Frequency-Reporting/data/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natashasoldin/Documents/Work/Sunrise Frequency Reporting/Sunrise-Frequency-Reporting/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C27B7D-72F9-8C4B-9657-A25FD6AEC945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6104D93-DB58-0C43-AA84-E70EE2984091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37180" yWindow="5400" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{38A25583-7701-1647-97E3-DC304504240B}"/>
+    <workbookView xWindow="37180" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{38A25583-7701-1647-97E3-DC304504240B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Current deliveries" sheetId="1" r:id="rId1"/>
+    <sheet name="Current deliveries" sheetId="3" r:id="rId1"/>
     <sheet name="Completed deliveries" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" iterateCount="1"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,16 +36,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>FREQUENCY REPORT</t>
+  </si>
+  <si>
+    <t>client_name</t>
+  </si>
+  <si>
+    <t>date_time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -54,8 +60,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="12"/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -82,13 +102,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -112,22 +139,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9CDFE74-0C6D-E734-80FF-F1EEDFB9A790}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F164AF-09B8-884D-A182-2E7D99A46F8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -143,7 +170,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="228600" y="50800"/>
+          <a:off x="177800" y="127000"/>
           <a:ext cx="4533900" cy="1524000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -161,15 +188,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>177800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -192,7 +219,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="228600" y="50800"/>
+          <a:off x="177800" y="127000"/>
           <a:ext cx="4533900" cy="1524000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -501,11 +528,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F94F693-DE8A-074D-9634-C231B96F9429}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC63E38F-1972-EF43-B9EA-2E28A018FDEC}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="A1:H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -526,22 +553,25 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2"/>
@@ -553,7 +583,9 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -581,9 +613,8 @@
       <c r="F8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:F8"/>
-    <mergeCell ref="G4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -594,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3419A2-BDD0-2541-8164-6EEEDA1FF00D}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,22 +647,25 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G3" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="H4" s="2"/>
@@ -643,7 +677,9 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -671,9 +707,8 @@
       <c r="F8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:F8"/>
-    <mergeCell ref="G4:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Began working on collection report incorporation, fixed multiple errors but still not finished
</commit_message>
<xml_diff>
--- a/assets/frequency_report_template.xlsx
+++ b/assets/frequency_report_template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natashasoldin/Documents/Work/Sunrise Frequency Reporting/Sunrise-Frequency-Reporting/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6104D93-DB58-0C43-AA84-E70EE2984091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B680BFD-9F62-CE4F-B818-A5E976179FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37180" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{38A25583-7701-1647-97E3-DC304504240B}"/>
+    <workbookView xWindow="37180" yWindow="5400" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{38A25583-7701-1647-97E3-DC304504240B}"/>
   </bookViews>
   <sheets>
     <sheet name="Current deliveries" sheetId="3" r:id="rId1"/>
     <sheet name="Completed deliveries" sheetId="2" r:id="rId2"/>
+    <sheet name="Collections" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>FREQUENCY REPORT</t>
   </si>
@@ -105,9 +106,6 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -116,6 +114,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -204,6 +205,55 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61EE0E61-C77F-AC42-9110-E917E0AABBE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="177800" y="127000"/>
+          <a:ext cx="4533900" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79241A31-0C1A-C24E-BFD7-737E74D5C9E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -531,86 +581,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC63E38F-1972-EF43-B9EA-2E28A018FDEC}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="5" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -632,79 +682,173 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="3" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="4" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="5" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2686334-EE8B-8548-AB56-EC0A88E76DCD}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>